<commit_message>
close #67 - Aggiornamento file excel e immagine
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/graficoGulpease.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/graficoGulpease.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65BAD32-FA19-4FD5-B443-1FFCA65F947F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9BF4D6-7EA8-4984-BF92-7E6A356A5ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3440947A-BDC3-41E2-B8C4-C01620109B14}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Indice Gulpease</t>
   </si>
@@ -102,13 +102,22 @@
   </si>
   <si>
     <t>VE_2020-12-22</t>
+  </si>
+  <si>
+    <t>Glossario</t>
+  </si>
+  <si>
+    <t>VE_2021-01-05</t>
+  </si>
+  <si>
+    <t>VI_2020-12-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +149,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -167,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -190,17 +205,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -382,9 +410,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -401,9 +429,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -411,30 +442,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$C$3:$C$9</c:f>
+              <c:f>Foglio1!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
+                <c:pt idx="7">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,9 +562,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -547,9 +581,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -557,10 +594,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$D$9</c:f>
+              <c:f>Foglio1!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -653,9 +690,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -672,9 +709,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -682,10 +722,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$E$3:$E$9</c:f>
+              <c:f>Foglio1!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -778,9 +818,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -797,9 +837,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -807,10 +850,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$F$3:$F$9</c:f>
+              <c:f>Foglio1!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -866,9 +909,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -885,9 +928,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -895,10 +941,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$G$3:$G$9</c:f>
+              <c:f>Foglio1!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -918,6 +964,9 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -961,9 +1010,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$B$3:$B$9</c:f>
+              <c:f>Foglio1!$B$3:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Analisi dei Requisiti</c:v>
                 </c:pt>
@@ -980,9 +1029,12 @@
                   <c:v>Studio di Fattibilità</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Verbali Esterni (Media)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Verbali Interni (Media)</c:v>
                 </c:pt>
               </c:strCache>
@@ -990,10 +1042,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$H$3:$H$9</c:f>
+              <c:f>Foglio1!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -1013,6 +1065,9 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -2116,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AECFA2-8686-4F57-8313-C78888B00A1F}">
-  <dimension ref="B2:H35"/>
+  <dimension ref="B2:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2129,7 +2184,7 @@
     <col min="7" max="7" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2152,12 +2207,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2169,12 +2224,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2186,12 +2241,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2203,12 +2258,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2220,12 +2275,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2236,32 +2291,40 @@
       <c r="H7" s="2">
         <v>80</v>
       </c>
+      <c r="J7" s="7">
+        <v>43</v>
+      </c>
+      <c r="N7" s="7">
+        <v>40</v>
+      </c>
+      <c r="O7" s="7">
+        <v>80</v>
+      </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2">
-        <f>_xlfn.CEILING.MATH(AVERAGE(C17:C21))</f>
-        <v>6</v>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7">
+        <v>59</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="G8" s="7">
         <v>40</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
-        <f>AVERAGE(C34:C35)</f>
-        <v>5</v>
+        <f>_xlfn.CEILING.MATH(AVERAGE(C34:C36))</f>
+        <v>60</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2273,10 +2336,28 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <f>_xlfn.CEILING.MATH(AVERAGE(C17:C22))</f>
+        <v>61</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>40</v>
+      </c>
+      <c r="H10" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F13" s="5"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2298,7 +2379,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="2">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2309,7 +2390,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2320,7 +2401,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="2">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2331,7 +2412,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2342,12 +2423,23 @@
         <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2">
+        <v>64</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>20</v>
@@ -2370,7 +2462,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="2">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2381,13 +2473,25 @@
         <v>22</v>
       </c>
       <c r="C35" s="2">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="2">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>